<commit_message>
"Changes dating back to YYYY-MM-DD"
</commit_message>
<xml_diff>
--- a/Documents/Sprint 1/burnUpChartSprint1.xlsx
+++ b/Documents/Sprint 1/burnUpChartSprint1.xlsx
@@ -57,11 +57,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -77,6 +78,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -198,7 +204,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -233,43 +239,8 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>Iteration0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Iteration1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Iteration2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Iteration3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Iteration4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Iteration5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Iteration6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Iteration7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Iteration8</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$10</c:f>
@@ -333,43 +304,8 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>Iteration0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Iteration1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Iteration2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Iteration3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Iteration4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Iteration5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Iteration6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Iteration7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Iteration8</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$C$2:$C$10</c:f>
@@ -407,11 +343,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="60639516"/>
-        <c:axId val="24907668"/>
+        <c:axId val="80510391"/>
+        <c:axId val="60706458"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="60639516"/>
+        <c:axId val="80510391"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -427,11 +363,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="24907668"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="60706458"/>
+        <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="24907668"/>
+        <c:axId val="60706458"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -456,8 +392,8 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="60639516"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="80510391"/>
+        <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -495,16 +431,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>16560</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>112680</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>9360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>86760</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>182520</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>151200</xdr:rowOff>
+      <xdr:rowOff>160200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -512,8 +448,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2454840" y="0"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="3363840" y="9360"/>
+        <a:ext cx="5759280" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">

</xml_diff>